<commit_message>
recop control, finished data call implementation
</commit_message>
<xml_diff>
--- a/control_isa.xlsx
+++ b/control_isa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\compsys701\uoa-cs701-2017-ajs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\uoa.auckland.ac.nz\engdfs\Home\klai054\compsys701\uoa-cs701-2017-ajs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -299,15 +299,9 @@
     <t>Data Call</t>
   </si>
   <si>
-    <t>D-Type: DPRR = 0; DPCR = 0</t>
-  </si>
-  <si>
     <t>D-Type: DPCR = Reg[RR2] &amp; (IR[15..0]/Reg[RR1]); IF BLOCKING THEN (DPC = 1)</t>
   </si>
   <si>
-    <t>D-Type: Reg[0] = DPRR[1..0]; M[DPRR[23..12]] = DPRR[1..0]; DPC = 0</t>
-  </si>
-  <si>
     <t>ID2</t>
   </si>
   <si>
@@ -327,6 +321,12 @@
   </si>
   <si>
     <t>DR</t>
+  </si>
+  <si>
+    <t>D-Type: Reg[0] = DPRR[1..0]; M[DPRR[23..12]] = DPRR[1..0]</t>
+  </si>
+  <si>
+    <t>D-Type: DPRR = 0; DPCR = 0]; DPC = 0</t>
   </si>
 </sst>
 </file>
@@ -839,6 +839,93 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -869,98 +956,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1252,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,22 +1264,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="107" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
       <c r="D1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="109" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="81"/>
-      <c r="G1" s="81"/>
-      <c r="H1" s="81"/>
-      <c r="I1" s="81"/>
-      <c r="J1" s="81"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
       <c r="K1" s="58"/>
       <c r="L1" s="29" t="s">
         <v>78</v>
@@ -1397,71 +1397,71 @@
         <v>37</v>
       </c>
       <c r="F2" s="71" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H2" s="71" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="113"/>
+      <c r="J2" s="81"/>
       <c r="K2" s="37"/>
       <c r="L2" s="30" t="s">
         <v>70</v>
       </c>
       <c r="M2" s="11"/>
-      <c r="N2" s="82" t="s">
+      <c r="N2" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="83"/>
+      <c r="O2" s="112"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="12"/>
-      <c r="R2" s="77" t="s">
+      <c r="R2" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="77"/>
-      <c r="T2" s="77" t="s">
+      <c r="S2" s="106"/>
+      <c r="T2" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="77"/>
-      <c r="V2" s="77"/>
-      <c r="W2" s="77"/>
-      <c r="X2" s="77"/>
-      <c r="Y2" s="77"/>
-      <c r="Z2" s="77" t="s">
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="106"/>
+      <c r="X2" s="106"/>
+      <c r="Y2" s="106"/>
+      <c r="Z2" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="77"/>
-      <c r="AC2" s="77"/>
-      <c r="AD2" s="77" t="s">
+      <c r="AA2" s="106"/>
+      <c r="AB2" s="106"/>
+      <c r="AC2" s="106"/>
+      <c r="AD2" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="77"/>
-      <c r="AF2" s="77"/>
-      <c r="AG2" s="77"/>
-      <c r="AH2" s="77" t="s">
+      <c r="AE2" s="106"/>
+      <c r="AF2" s="106"/>
+      <c r="AG2" s="106"/>
+      <c r="AH2" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="77"/>
-      <c r="AJ2" s="77"/>
-      <c r="AK2" s="77"/>
-      <c r="AL2" s="77"/>
-      <c r="AM2" s="77"/>
-      <c r="AN2" s="77"/>
-      <c r="AO2" s="77"/>
-      <c r="AP2" s="77"/>
-      <c r="AQ2" s="77"/>
-      <c r="AR2" s="77"/>
-      <c r="AS2" s="77"/>
-      <c r="AT2" s="77"/>
-      <c r="AU2" s="77"/>
-      <c r="AV2" s="77"/>
-      <c r="AW2" s="77"/>
+      <c r="AI2" s="106"/>
+      <c r="AJ2" s="106"/>
+      <c r="AK2" s="106"/>
+      <c r="AL2" s="106"/>
+      <c r="AM2" s="106"/>
+      <c r="AN2" s="106"/>
+      <c r="AO2" s="106"/>
+      <c r="AP2" s="106"/>
+      <c r="AQ2" s="106"/>
+      <c r="AR2" s="106"/>
+      <c r="AS2" s="106"/>
+      <c r="AT2" s="106"/>
+      <c r="AU2" s="106"/>
+      <c r="AV2" s="106"/>
+      <c r="AW2" s="106"/>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
@@ -1478,7 +1478,7 @@
         <v>37</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>39</v>
@@ -1488,10 +1488,10 @@
       <c r="J3" s="11"/>
       <c r="K3" s="35"/>
       <c r="L3" s="31"/>
-      <c r="N3" s="88" t="s">
+      <c r="N3" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="89"/>
+      <c r="O3" s="114"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
@@ -1511,13 +1511,13 @@
         <v>37</v>
       </c>
       <c r="F4" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G4" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H4" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>39</v>
@@ -1525,10 +1525,10 @@
       <c r="J4" s="53"/>
       <c r="K4" s="54"/>
       <c r="L4" s="31"/>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="89"/>
+      <c r="O4" s="114"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
@@ -1548,7 +1548,7 @@
         <v>37</v>
       </c>
       <c r="F5" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G5" s="14" t="s">
         <v>39</v>
@@ -1558,10 +1558,10 @@
       <c r="J5" s="11"/>
       <c r="K5" s="35"/>
       <c r="L5" s="31"/>
-      <c r="N5" s="88" t="s">
+      <c r="N5" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="89"/>
+      <c r="O5" s="114"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
@@ -1582,13 +1582,13 @@
         <v>37</v>
       </c>
       <c r="F6" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H6" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>39</v>
@@ -1596,10 +1596,10 @@
       <c r="J6" s="53"/>
       <c r="K6" s="54"/>
       <c r="L6" s="31"/>
-      <c r="N6" s="88" t="s">
+      <c r="N6" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="O6" s="89"/>
+      <c r="O6" s="114"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
@@ -1620,7 +1620,7 @@
         <v>37</v>
       </c>
       <c r="F7" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>39</v>
@@ -1630,10 +1630,10 @@
       <c r="J7" s="11"/>
       <c r="K7" s="35"/>
       <c r="L7" s="31"/>
-      <c r="N7" s="88" t="s">
+      <c r="N7" s="113" t="s">
         <v>47</v>
       </c>
-      <c r="O7" s="89"/>
+      <c r="O7" s="114"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
@@ -1654,13 +1654,13 @@
         <v>37</v>
       </c>
       <c r="F8" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H8" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>39</v>
@@ -1668,10 +1668,10 @@
       <c r="J8" s="53"/>
       <c r="K8" s="54"/>
       <c r="L8" s="31"/>
-      <c r="N8" s="84" t="s">
+      <c r="N8" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="O8" s="85"/>
+      <c r="O8" s="94"/>
       <c r="P8" s="11"/>
       <c r="Q8" s="12"/>
       <c r="R8" s="12"/>
@@ -1692,13 +1692,13 @@
         <v>37</v>
       </c>
       <c r="F9" s="73" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>38</v>
       </c>
       <c r="H9" s="73" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>39</v>
@@ -1706,10 +1706,10 @@
       <c r="J9" s="57"/>
       <c r="K9" s="55"/>
       <c r="L9" s="31"/>
-      <c r="N9" s="86" t="s">
+      <c r="N9" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="O9" s="87"/>
+      <c r="O9" s="98"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
@@ -1730,13 +1730,13 @@
         <v>37</v>
       </c>
       <c r="F10" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G10" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H10" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>39</v>
@@ -1746,10 +1746,10 @@
       <c r="L10" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="N10" s="96" t="s">
+      <c r="N10" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="97"/>
+      <c r="O10" s="90"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
@@ -1770,22 +1770,22 @@
         <v>37</v>
       </c>
       <c r="F11" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G11" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="11"/>
       <c r="K11" s="35"/>
       <c r="L11" s="51"/>
-      <c r="N11" s="98" t="s">
+      <c r="N11" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="99"/>
+      <c r="O11" s="92"/>
       <c r="P11" s="11"/>
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
@@ -1805,26 +1805,26 @@
         <v>37</v>
       </c>
       <c r="F12" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G12" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H12" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>39</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K12" s="54"/>
       <c r="L12" s="51"/>
-      <c r="N12" s="84" t="s">
+      <c r="N12" s="93" t="s">
         <v>52</v>
       </c>
-      <c r="O12" s="85"/>
+      <c r="O12" s="94"/>
       <c r="P12" s="11"/>
       <c r="R12" s="12"/>
       <c r="S12" s="12"/>
@@ -1844,13 +1844,13 @@
         <v>37</v>
       </c>
       <c r="F13" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H13" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>39</v>
@@ -1858,10 +1858,10 @@
       <c r="J13" s="11"/>
       <c r="K13" s="35"/>
       <c r="L13" s="51"/>
-      <c r="N13" s="86" t="s">
+      <c r="N13" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="O13" s="87"/>
+      <c r="O13" s="98"/>
       <c r="P13" s="11"/>
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
@@ -1881,7 +1881,7 @@
         <v>37</v>
       </c>
       <c r="F14" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G14" s="14" t="s">
         <v>39</v>
@@ -1891,10 +1891,10 @@
       <c r="J14" s="11"/>
       <c r="K14" s="35"/>
       <c r="L14" s="51"/>
-      <c r="N14" s="102" t="s">
+      <c r="N14" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="O14" s="103"/>
+      <c r="O14" s="100"/>
       <c r="P14" s="11"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
@@ -1914,13 +1914,13 @@
         <v>37</v>
       </c>
       <c r="F15" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G15" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H15" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I15" s="14" t="s">
         <v>39</v>
@@ -1928,10 +1928,10 @@
       <c r="J15" s="11"/>
       <c r="K15" s="35"/>
       <c r="L15" s="51"/>
-      <c r="N15" s="104" t="s">
+      <c r="N15" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="O15" s="105"/>
+      <c r="O15" s="102"/>
       <c r="P15" s="11"/>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
@@ -1951,26 +1951,26 @@
         <v>37</v>
       </c>
       <c r="F16" s="71" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>38</v>
       </c>
       <c r="H16" s="71" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>39</v>
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="36"/>
-      <c r="L16" s="74" t="s">
+      <c r="L16" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="N16" s="104" t="s">
+      <c r="N16" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="O16" s="105"/>
+      <c r="O16" s="102"/>
       <c r="P16" s="11"/>
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
@@ -1990,7 +1990,7 @@
         <v>37</v>
       </c>
       <c r="F17" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G17" s="14" t="s">
         <v>39</v>
@@ -1999,11 +1999,11 @@
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="35"/>
-      <c r="L17" s="75"/>
-      <c r="N17" s="104" t="s">
+      <c r="L17" s="104"/>
+      <c r="N17" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O17" s="105"/>
+      <c r="O17" s="102"/>
       <c r="P17" s="11"/>
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
@@ -2021,24 +2021,24 @@
         <v>37</v>
       </c>
       <c r="F18" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G18" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H18" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>39</v>
       </c>
       <c r="J18" s="53"/>
       <c r="K18" s="54"/>
-      <c r="L18" s="76"/>
-      <c r="N18" s="100" t="s">
+      <c r="L18" s="105"/>
+      <c r="N18" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="O18" s="101"/>
+      <c r="O18" s="96"/>
       <c r="P18" s="11"/>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
@@ -2058,26 +2058,26 @@
         <v>37</v>
       </c>
       <c r="F19" s="71" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>39</v>
       </c>
       <c r="H19" s="60" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I19" s="61" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J19" s="7"/>
       <c r="K19" s="37"/>
       <c r="L19" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="N19" s="86" t="s">
+      <c r="N19" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="O19" s="87"/>
+      <c r="O19" s="98"/>
       <c r="P19" s="11"/>
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
@@ -2097,28 +2097,28 @@
         <v>37</v>
       </c>
       <c r="F20" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H20" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>39</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K20" s="62" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L20" s="64"/>
-      <c r="N20" s="86" t="s">
+      <c r="N20" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="O20" s="87"/>
+      <c r="O20" s="98"/>
       <c r="P20" s="11"/>
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
@@ -2138,24 +2138,24 @@
         <v>37</v>
       </c>
       <c r="F21" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I21" s="63" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J21" s="11"/>
       <c r="K21" s="35"/>
       <c r="L21" s="64"/>
-      <c r="N21" s="86" t="s">
+      <c r="N21" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="O21" s="87"/>
+      <c r="O21" s="98"/>
       <c r="P21" s="11"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
@@ -2175,28 +2175,28 @@
         <v>37</v>
       </c>
       <c r="F22" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G22" s="16" t="s">
         <v>38</v>
       </c>
       <c r="H22" s="72" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I22" s="14" t="s">
         <v>39</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K22" s="62" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L22" s="64"/>
-      <c r="N22" s="94" t="s">
+      <c r="N22" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="O22" s="95"/>
+      <c r="O22" s="88"/>
       <c r="P22" s="11"/>
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
@@ -2210,30 +2210,30 @@
       <c r="D23" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="107" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="108" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" s="109" t="s">
+      <c r="E23" s="75" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="G23" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="108" t="s">
-        <v>94</v>
-      </c>
-      <c r="I23" s="110" t="s">
-        <v>39</v>
-      </c>
-      <c r="J23" s="111"/>
-      <c r="K23" s="112"/>
+      <c r="H23" s="76" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" s="79"/>
+      <c r="K23" s="80"/>
       <c r="L23" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="N23" s="90" t="s">
+      <c r="N23" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="O23" s="91"/>
+      <c r="O23" s="84"/>
       <c r="P23" s="11"/>
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
@@ -2251,7 +2251,7 @@
         <v>37</v>
       </c>
       <c r="F24" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G24" s="14" t="s">
         <v>39</v>
@@ -2263,10 +2263,10 @@
       <c r="L24" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="N24" s="92" t="s">
+      <c r="N24" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="O24" s="93"/>
+      <c r="O24" s="86"/>
       <c r="P24" s="11"/>
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
@@ -2284,7 +2284,7 @@
         <v>37</v>
       </c>
       <c r="F25" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G25" s="14" t="s">
         <v>39</v>
@@ -2294,10 +2294,10 @@
       <c r="J25" s="11"/>
       <c r="K25" s="35"/>
       <c r="L25" s="67"/>
-      <c r="N25" s="94" t="s">
+      <c r="N25" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="O25" s="95"/>
+      <c r="O25" s="88"/>
       <c r="P25" s="11"/>
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
@@ -2315,7 +2315,7 @@
         <v>37</v>
       </c>
       <c r="F26" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G26" s="14" t="s">
         <v>39</v>
@@ -2344,12 +2344,12 @@
         <v>37</v>
       </c>
       <c r="F27" s="73" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G27" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H27" s="106"/>
+      <c r="H27" s="74"/>
       <c r="I27" s="20"/>
       <c r="J27" s="20"/>
       <c r="K27" s="32"/>
@@ -2374,7 +2374,7 @@
         <v>37</v>
       </c>
       <c r="F28" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G28" s="14" t="s">
         <v>39</v>
@@ -2406,7 +2406,7 @@
         <v>37</v>
       </c>
       <c r="F29" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G29" s="14" t="s">
         <v>39</v>
@@ -2436,7 +2436,7 @@
         <v>37</v>
       </c>
       <c r="F30" s="72" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G30" s="14" t="s">
         <v>39</v>
@@ -2466,12 +2466,12 @@
         <v>37</v>
       </c>
       <c r="F31" s="73" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H31" s="106"/>
+      <c r="H31" s="74"/>
       <c r="I31" s="20"/>
       <c r="J31" s="20"/>
       <c r="K31" s="32"/>
@@ -2496,9 +2496,9 @@
         <v>37</v>
       </c>
       <c r="F32" s="73" t="s">
-        <v>95</v>
-      </c>
-      <c r="G32" s="106"/>
+        <v>93</v>
+      </c>
+      <c r="G32" s="74"/>
       <c r="H32" s="57"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -2526,18 +2526,18 @@
         <v>37</v>
       </c>
       <c r="F33" s="73" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G33" s="18" t="s">
         <v>38</v>
       </c>
       <c r="H33" s="73" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I33" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J33" s="114"/>
+      <c r="J33" s="82"/>
       <c r="K33" s="55"/>
       <c r="L33" s="70" t="s">
         <v>70</v>
@@ -2562,13 +2562,13 @@
         <v>37</v>
       </c>
       <c r="F34" s="73" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G34" s="18" t="s">
         <v>38</v>
       </c>
       <c r="H34" s="73" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I34" s="19" t="s">
         <v>39</v>
@@ -2681,7 +2681,7 @@
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B43" s="23"/>
       <c r="C43" s="23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D43" s="23"/>
     </row>
@@ -2708,38 +2708,54 @@
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C47" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D47" s="23"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B48" s="25" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="23"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C49" s="23" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D49" s="23"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C50" s="23"/>
       <c r="D50" s="23"/>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C51" s="23" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="D51" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AW2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:Y2"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
     <mergeCell ref="N23:O23"/>
     <mergeCell ref="N24:O24"/>
     <mergeCell ref="N25:O25"/>
@@ -2756,22 +2772,6 @@
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="N17:O17"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:Y2"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
recop control test benching
</commit_message>
<xml_diff>
--- a/control_isa.xlsx
+++ b/control_isa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\uoa.auckland.ac.nz\engdfs\Home\klai054\compsys701\uoa-cs701-2017-ajs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\compsys701\uoa-cs701-2017-ajs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -866,6 +866,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -896,24 +944,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -924,42 +960,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1252,8 +1252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,22 +1264,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="87" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
       <c r="D1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="109" t="s">
+      <c r="E1" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
       <c r="K1" s="58"/>
       <c r="L1" s="29" t="s">
         <v>78</v>
@@ -1414,54 +1414,54 @@
         <v>70</v>
       </c>
       <c r="M2" s="11"/>
-      <c r="N2" s="111" t="s">
+      <c r="N2" s="91" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="112"/>
+      <c r="O2" s="92"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="12"/>
-      <c r="R2" s="106" t="s">
+      <c r="R2" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="106"/>
-      <c r="T2" s="106" t="s">
+      <c r="S2" s="86"/>
+      <c r="T2" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="106"/>
-      <c r="V2" s="106"/>
-      <c r="W2" s="106"/>
-      <c r="X2" s="106"/>
-      <c r="Y2" s="106"/>
-      <c r="Z2" s="106" t="s">
+      <c r="U2" s="86"/>
+      <c r="V2" s="86"/>
+      <c r="W2" s="86"/>
+      <c r="X2" s="86"/>
+      <c r="Y2" s="86"/>
+      <c r="Z2" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="106"/>
-      <c r="AB2" s="106"/>
-      <c r="AC2" s="106"/>
-      <c r="AD2" s="106" t="s">
+      <c r="AA2" s="86"/>
+      <c r="AB2" s="86"/>
+      <c r="AC2" s="86"/>
+      <c r="AD2" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="106"/>
-      <c r="AF2" s="106"/>
-      <c r="AG2" s="106"/>
-      <c r="AH2" s="106" t="s">
+      <c r="AE2" s="86"/>
+      <c r="AF2" s="86"/>
+      <c r="AG2" s="86"/>
+      <c r="AH2" s="86" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="106"/>
-      <c r="AJ2" s="106"/>
-      <c r="AK2" s="106"/>
-      <c r="AL2" s="106"/>
-      <c r="AM2" s="106"/>
-      <c r="AN2" s="106"/>
-      <c r="AO2" s="106"/>
-      <c r="AP2" s="106"/>
-      <c r="AQ2" s="106"/>
-      <c r="AR2" s="106"/>
-      <c r="AS2" s="106"/>
-      <c r="AT2" s="106"/>
-      <c r="AU2" s="106"/>
-      <c r="AV2" s="106"/>
-      <c r="AW2" s="106"/>
+      <c r="AI2" s="86"/>
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="86"/>
+      <c r="AL2" s="86"/>
+      <c r="AM2" s="86"/>
+      <c r="AN2" s="86"/>
+      <c r="AO2" s="86"/>
+      <c r="AP2" s="86"/>
+      <c r="AQ2" s="86"/>
+      <c r="AR2" s="86"/>
+      <c r="AS2" s="86"/>
+      <c r="AT2" s="86"/>
+      <c r="AU2" s="86"/>
+      <c r="AV2" s="86"/>
+      <c r="AW2" s="86"/>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
@@ -1488,10 +1488,10 @@
       <c r="J3" s="11"/>
       <c r="K3" s="35"/>
       <c r="L3" s="31"/>
-      <c r="N3" s="113" t="s">
+      <c r="N3" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="114"/>
+      <c r="O3" s="98"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
@@ -1525,10 +1525,10 @@
       <c r="J4" s="53"/>
       <c r="K4" s="54"/>
       <c r="L4" s="31"/>
-      <c r="N4" s="113" t="s">
+      <c r="N4" s="97" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="114"/>
+      <c r="O4" s="98"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
@@ -1558,10 +1558,10 @@
       <c r="J5" s="11"/>
       <c r="K5" s="35"/>
       <c r="L5" s="31"/>
-      <c r="N5" s="113" t="s">
+      <c r="N5" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="114"/>
+      <c r="O5" s="98"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
@@ -1596,10 +1596,10 @@
       <c r="J6" s="53"/>
       <c r="K6" s="54"/>
       <c r="L6" s="31"/>
-      <c r="N6" s="113" t="s">
+      <c r="N6" s="97" t="s">
         <v>46</v>
       </c>
-      <c r="O6" s="114"/>
+      <c r="O6" s="98"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
@@ -1630,10 +1630,10 @@
       <c r="J7" s="11"/>
       <c r="K7" s="35"/>
       <c r="L7" s="31"/>
-      <c r="N7" s="113" t="s">
+      <c r="N7" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="O7" s="114"/>
+      <c r="O7" s="98"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="45" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E8" s="34" t="s">
         <v>37</v>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="45" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E9" s="59" t="s">
         <v>37</v>
@@ -1706,10 +1706,10 @@
       <c r="J9" s="57"/>
       <c r="K9" s="55"/>
       <c r="L9" s="31"/>
-      <c r="N9" s="97" t="s">
+      <c r="N9" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="O9" s="98"/>
+      <c r="O9" s="96"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
@@ -1746,10 +1746,10 @@
       <c r="L10" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="N10" s="89" t="s">
+      <c r="N10" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="90"/>
+      <c r="O10" s="106"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
@@ -1782,10 +1782,10 @@
       <c r="J11" s="11"/>
       <c r="K11" s="35"/>
       <c r="L11" s="51"/>
-      <c r="N11" s="91" t="s">
+      <c r="N11" s="107" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="92"/>
+      <c r="O11" s="108"/>
       <c r="P11" s="11"/>
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
@@ -1858,10 +1858,10 @@
       <c r="J13" s="11"/>
       <c r="K13" s="35"/>
       <c r="L13" s="51"/>
-      <c r="N13" s="97" t="s">
+      <c r="N13" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="O13" s="98"/>
+      <c r="O13" s="96"/>
       <c r="P13" s="11"/>
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
@@ -1891,10 +1891,10 @@
       <c r="J14" s="11"/>
       <c r="K14" s="35"/>
       <c r="L14" s="51"/>
-      <c r="N14" s="99" t="s">
+      <c r="N14" s="111" t="s">
         <v>54</v>
       </c>
-      <c r="O14" s="100"/>
+      <c r="O14" s="112"/>
       <c r="P14" s="11"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
@@ -1928,10 +1928,10 @@
       <c r="J15" s="11"/>
       <c r="K15" s="35"/>
       <c r="L15" s="51"/>
-      <c r="N15" s="101" t="s">
+      <c r="N15" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="O15" s="102"/>
+      <c r="O15" s="114"/>
       <c r="P15" s="11"/>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
@@ -1964,13 +1964,13 @@
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="36"/>
-      <c r="L16" s="103" t="s">
+      <c r="L16" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="N16" s="101" t="s">
+      <c r="N16" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="O16" s="102"/>
+      <c r="O16" s="114"/>
       <c r="P16" s="11"/>
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
@@ -1999,11 +1999,11 @@
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="35"/>
-      <c r="L17" s="104"/>
-      <c r="N17" s="101" t="s">
+      <c r="L17" s="84"/>
+      <c r="N17" s="113" t="s">
         <v>57</v>
       </c>
-      <c r="O17" s="102"/>
+      <c r="O17" s="114"/>
       <c r="P17" s="11"/>
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
@@ -2034,11 +2034,11 @@
       </c>
       <c r="J18" s="53"/>
       <c r="K18" s="54"/>
-      <c r="L18" s="105"/>
-      <c r="N18" s="95" t="s">
+      <c r="L18" s="85"/>
+      <c r="N18" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="O18" s="96"/>
+      <c r="O18" s="110"/>
       <c r="P18" s="11"/>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
@@ -2074,10 +2074,10 @@
       <c r="L19" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="N19" s="97" t="s">
+      <c r="N19" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="O19" s="98"/>
+      <c r="O19" s="96"/>
       <c r="P19" s="11"/>
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
@@ -2115,10 +2115,10 @@
         <v>98</v>
       </c>
       <c r="L20" s="64"/>
-      <c r="N20" s="97" t="s">
+      <c r="N20" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="O20" s="98"/>
+      <c r="O20" s="96"/>
       <c r="P20" s="11"/>
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
@@ -2152,10 +2152,10 @@
       <c r="J21" s="11"/>
       <c r="K21" s="35"/>
       <c r="L21" s="64"/>
-      <c r="N21" s="97" t="s">
+      <c r="N21" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="O21" s="98"/>
+      <c r="O21" s="96"/>
       <c r="P21" s="11"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
@@ -2193,10 +2193,10 @@
         <v>98</v>
       </c>
       <c r="L22" s="64"/>
-      <c r="N22" s="87" t="s">
+      <c r="N22" s="103" t="s">
         <v>62</v>
       </c>
-      <c r="O22" s="88"/>
+      <c r="O22" s="104"/>
       <c r="P22" s="11"/>
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
@@ -2230,10 +2230,10 @@
       <c r="L23" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="N23" s="83" t="s">
+      <c r="N23" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="O23" s="84"/>
+      <c r="O23" s="100"/>
       <c r="P23" s="11"/>
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
@@ -2263,10 +2263,10 @@
       <c r="L24" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="N24" s="85" t="s">
+      <c r="N24" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="O24" s="86"/>
+      <c r="O24" s="102"/>
       <c r="P24" s="11"/>
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
@@ -2294,10 +2294,10 @@
       <c r="J25" s="11"/>
       <c r="K25" s="35"/>
       <c r="L25" s="67"/>
-      <c r="N25" s="87" t="s">
+      <c r="N25" s="103" t="s">
         <v>65</v>
       </c>
-      <c r="O25" s="88"/>
+      <c r="O25" s="104"/>
       <c r="P25" s="11"/>
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
@@ -2740,6 +2740,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N17:O17"/>
     <mergeCell ref="L16:L18"/>
     <mergeCell ref="AD2:AG2"/>
     <mergeCell ref="AH2:AW2"/>
@@ -2756,22 +2772,6 @@
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="N7:O7"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="N10:O10"/>
-    <mergeCell ref="N11:O11"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N17:O17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
walao we da best, also everything works
</commit_message>
<xml_diff>
--- a/control_isa.xlsx
+++ b/control_isa.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="105">
   <si>
     <t>AND</t>
   </si>
@@ -327,6 +327,18 @@
   </si>
   <si>
     <t>D-Type: DPRR = 0; DPCR = 0]; DPC = 0</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>JP</t>
   </si>
 </sst>
 </file>
@@ -866,6 +878,66 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -896,70 +968,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1252,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16:O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1264,22 +1276,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="107" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="108"/>
       <c r="D1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="109" t="s">
         <v>79</v>
       </c>
-      <c r="F1" s="90"/>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
+      <c r="F1" s="110"/>
+      <c r="G1" s="110"/>
+      <c r="H1" s="110"/>
+      <c r="I1" s="110"/>
+      <c r="J1" s="110"/>
       <c r="K1" s="58"/>
       <c r="L1" s="29" t="s">
         <v>78</v>
@@ -1414,54 +1426,54 @@
         <v>70</v>
       </c>
       <c r="M2" s="11"/>
-      <c r="N2" s="91" t="s">
+      <c r="N2" s="111" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="92"/>
+      <c r="O2" s="112"/>
       <c r="P2" s="11"/>
       <c r="Q2" s="12"/>
-      <c r="R2" s="86" t="s">
+      <c r="R2" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="86"/>
-      <c r="T2" s="86" t="s">
+      <c r="S2" s="106"/>
+      <c r="T2" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="U2" s="86"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="86"/>
-      <c r="X2" s="86"/>
-      <c r="Y2" s="86"/>
-      <c r="Z2" s="86" t="s">
+      <c r="U2" s="106"/>
+      <c r="V2" s="106"/>
+      <c r="W2" s="106"/>
+      <c r="X2" s="106"/>
+      <c r="Y2" s="106"/>
+      <c r="Z2" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="AA2" s="86"/>
-      <c r="AB2" s="86"/>
-      <c r="AC2" s="86"/>
-      <c r="AD2" s="86" t="s">
+      <c r="AA2" s="106"/>
+      <c r="AB2" s="106"/>
+      <c r="AC2" s="106"/>
+      <c r="AD2" s="106" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="86"/>
-      <c r="AF2" s="86"/>
-      <c r="AG2" s="86"/>
-      <c r="AH2" s="86" t="s">
+      <c r="AE2" s="106"/>
+      <c r="AF2" s="106"/>
+      <c r="AG2" s="106"/>
+      <c r="AH2" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="86"/>
-      <c r="AJ2" s="86"/>
-      <c r="AK2" s="86"/>
-      <c r="AL2" s="86"/>
-      <c r="AM2" s="86"/>
-      <c r="AN2" s="86"/>
-      <c r="AO2" s="86"/>
-      <c r="AP2" s="86"/>
-      <c r="AQ2" s="86"/>
-      <c r="AR2" s="86"/>
-      <c r="AS2" s="86"/>
-      <c r="AT2" s="86"/>
-      <c r="AU2" s="86"/>
-      <c r="AV2" s="86"/>
-      <c r="AW2" s="86"/>
+      <c r="AI2" s="106"/>
+      <c r="AJ2" s="106"/>
+      <c r="AK2" s="106"/>
+      <c r="AL2" s="106"/>
+      <c r="AM2" s="106"/>
+      <c r="AN2" s="106"/>
+      <c r="AO2" s="106"/>
+      <c r="AP2" s="106"/>
+      <c r="AQ2" s="106"/>
+      <c r="AR2" s="106"/>
+      <c r="AS2" s="106"/>
+      <c r="AT2" s="106"/>
+      <c r="AU2" s="106"/>
+      <c r="AV2" s="106"/>
+      <c r="AW2" s="106"/>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
@@ -1488,10 +1500,10 @@
       <c r="J3" s="11"/>
       <c r="K3" s="35"/>
       <c r="L3" s="31"/>
-      <c r="N3" s="97" t="s">
+      <c r="N3" s="113" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="98"/>
+      <c r="O3" s="114"/>
       <c r="P3" s="11"/>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
@@ -1525,10 +1537,10 @@
       <c r="J4" s="53"/>
       <c r="K4" s="54"/>
       <c r="L4" s="31"/>
-      <c r="N4" s="97" t="s">
+      <c r="N4" s="113" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="98"/>
+      <c r="O4" s="114"/>
       <c r="P4" s="11"/>
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
@@ -1558,10 +1570,10 @@
       <c r="J5" s="11"/>
       <c r="K5" s="35"/>
       <c r="L5" s="31"/>
-      <c r="N5" s="97" t="s">
+      <c r="N5" s="113" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="98"/>
+      <c r="O5" s="114"/>
       <c r="P5" s="11"/>
       <c r="Q5" s="12"/>
       <c r="R5" s="12"/>
@@ -1596,10 +1608,10 @@
       <c r="J6" s="53"/>
       <c r="K6" s="54"/>
       <c r="L6" s="31"/>
-      <c r="N6" s="97" t="s">
+      <c r="N6" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="O6" s="98"/>
+      <c r="O6" s="114"/>
       <c r="P6" s="11"/>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
@@ -1630,10 +1642,10 @@
       <c r="J7" s="11"/>
       <c r="K7" s="35"/>
       <c r="L7" s="31"/>
-      <c r="N7" s="97" t="s">
+      <c r="N7" s="113" t="s">
         <v>47</v>
       </c>
-      <c r="O7" s="98"/>
+      <c r="O7" s="114"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="12"/>
       <c r="R7" s="12"/>
@@ -1706,10 +1718,10 @@
       <c r="J9" s="57"/>
       <c r="K9" s="55"/>
       <c r="L9" s="31"/>
-      <c r="N9" s="95" t="s">
+      <c r="N9" s="97" t="s">
         <v>49</v>
       </c>
-      <c r="O9" s="96"/>
+      <c r="O9" s="98"/>
       <c r="P9" s="11"/>
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
@@ -1739,17 +1751,17 @@
         <v>92</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="35"/>
       <c r="L10" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="N10" s="105" t="s">
+      <c r="N10" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="O10" s="106"/>
+      <c r="O10" s="90"/>
       <c r="P10" s="11"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
@@ -1773,19 +1785,19 @@
         <v>93</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="I11" s="12"/>
       <c r="J11" s="11"/>
       <c r="K11" s="35"/>
       <c r="L11" s="51"/>
-      <c r="N11" s="107" t="s">
+      <c r="N11" s="91" t="s">
         <v>51</v>
       </c>
-      <c r="O11" s="108"/>
+      <c r="O11" s="92"/>
       <c r="P11" s="11"/>
       <c r="R11" s="12"/>
       <c r="S11" s="12"/>
@@ -1814,10 +1826,10 @@
         <v>92</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>39</v>
+        <v>101</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="K12" s="54"/>
       <c r="L12" s="51"/>
@@ -1853,15 +1865,15 @@
         <v>92</v>
       </c>
       <c r="I13" s="14" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="35"/>
       <c r="L13" s="51"/>
-      <c r="N13" s="95" t="s">
+      <c r="N13" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="O13" s="96"/>
+      <c r="O13" s="98"/>
       <c r="P13" s="11"/>
       <c r="R13" s="12"/>
       <c r="S13" s="12"/>
@@ -1884,17 +1896,17 @@
         <v>93</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
       <c r="K14" s="35"/>
       <c r="L14" s="51"/>
-      <c r="N14" s="111" t="s">
+      <c r="N14" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="O14" s="112"/>
+      <c r="O14" s="100"/>
       <c r="P14" s="11"/>
       <c r="R14" s="12"/>
       <c r="S14" s="12"/>
@@ -1923,15 +1935,15 @@
         <v>92</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="35"/>
       <c r="L15" s="51"/>
-      <c r="N15" s="113" t="s">
+      <c r="N15" s="101" t="s">
         <v>55</v>
       </c>
-      <c r="O15" s="114"/>
+      <c r="O15" s="102"/>
       <c r="P15" s="11"/>
       <c r="R15" s="12"/>
       <c r="S15" s="12"/>
@@ -1960,17 +1972,17 @@
         <v>92</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J16" s="17"/>
       <c r="K16" s="36"/>
-      <c r="L16" s="83" t="s">
+      <c r="L16" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="N16" s="113" t="s">
+      <c r="N16" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="O16" s="114"/>
+      <c r="O16" s="102"/>
       <c r="P16" s="11"/>
       <c r="R16" s="12"/>
       <c r="S16" s="12"/>
@@ -1993,17 +2005,17 @@
         <v>93</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="11"/>
       <c r="J17" s="11"/>
       <c r="K17" s="35"/>
-      <c r="L17" s="84"/>
-      <c r="N17" s="113" t="s">
+      <c r="L17" s="104"/>
+      <c r="N17" s="101" t="s">
         <v>57</v>
       </c>
-      <c r="O17" s="114"/>
+      <c r="O17" s="102"/>
       <c r="P17" s="11"/>
       <c r="R17" s="12"/>
       <c r="S17" s="12"/>
@@ -2030,15 +2042,15 @@
         <v>92</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J18" s="53"/>
       <c r="K18" s="54"/>
-      <c r="L18" s="85"/>
-      <c r="N18" s="109" t="s">
+      <c r="L18" s="105"/>
+      <c r="N18" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="O18" s="110"/>
+      <c r="O18" s="96"/>
       <c r="P18" s="11"/>
       <c r="R18" s="12"/>
       <c r="S18" s="12"/>
@@ -2061,7 +2073,7 @@
         <v>93</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="H19" s="60" t="s">
         <v>97</v>
@@ -2074,10 +2086,10 @@
       <c r="L19" s="64" t="s">
         <v>89</v>
       </c>
-      <c r="N19" s="95" t="s">
+      <c r="N19" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="O19" s="96"/>
+      <c r="O19" s="98"/>
       <c r="P19" s="11"/>
       <c r="R19" s="12"/>
       <c r="S19" s="12"/>
@@ -2106,7 +2118,7 @@
         <v>92</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="J20" s="15" t="s">
         <v>97</v>
@@ -2115,10 +2127,10 @@
         <v>98</v>
       </c>
       <c r="L20" s="64"/>
-      <c r="N20" s="95" t="s">
+      <c r="N20" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="O20" s="96"/>
+      <c r="O20" s="98"/>
       <c r="P20" s="11"/>
       <c r="R20" s="12"/>
       <c r="S20" s="12"/>
@@ -2141,7 +2153,7 @@
         <v>93</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="H21" s="15" t="s">
         <v>97</v>
@@ -2152,10 +2164,10 @@
       <c r="J21" s="11"/>
       <c r="K21" s="35"/>
       <c r="L21" s="64"/>
-      <c r="N21" s="95" t="s">
+      <c r="N21" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="O21" s="96"/>
+      <c r="O21" s="98"/>
       <c r="P21" s="11"/>
       <c r="R21" s="12"/>
       <c r="S21" s="12"/>
@@ -2184,7 +2196,7 @@
         <v>92</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="J22" s="15" t="s">
         <v>97</v>
@@ -2193,10 +2205,10 @@
         <v>98</v>
       </c>
       <c r="L22" s="64"/>
-      <c r="N22" s="103" t="s">
+      <c r="N22" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="O22" s="104"/>
+      <c r="O22" s="88"/>
       <c r="P22" s="11"/>
       <c r="R22" s="12"/>
       <c r="S22" s="12"/>
@@ -2223,17 +2235,17 @@
         <v>92</v>
       </c>
       <c r="I23" s="78" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="J23" s="79"/>
       <c r="K23" s="80"/>
       <c r="L23" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="N23" s="99" t="s">
+      <c r="N23" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="O23" s="100"/>
+      <c r="O23" s="84"/>
       <c r="P23" s="11"/>
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
@@ -2263,10 +2275,10 @@
       <c r="L24" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="N24" s="101" t="s">
+      <c r="N24" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="O24" s="102"/>
+      <c r="O24" s="86"/>
       <c r="P24" s="11"/>
       <c r="R24" s="12"/>
       <c r="S24" s="12"/>
@@ -2294,10 +2306,10 @@
       <c r="J25" s="11"/>
       <c r="K25" s="35"/>
       <c r="L25" s="67"/>
-      <c r="N25" s="103" t="s">
+      <c r="N25" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="O25" s="104"/>
+      <c r="O25" s="88"/>
       <c r="P25" s="11"/>
       <c r="R25" s="12"/>
       <c r="S25" s="12"/>
@@ -2377,7 +2389,7 @@
         <v>93</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="11"/>
@@ -2409,7 +2421,7 @@
         <v>93</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="11"/>
@@ -2439,7 +2451,7 @@
         <v>93</v>
       </c>
       <c r="G30" s="14" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="11"/>
@@ -2469,7 +2481,7 @@
         <v>93</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="H31" s="74"/>
       <c r="I31" s="20"/>
@@ -2498,7 +2510,9 @@
       <c r="F32" s="73" t="s">
         <v>93</v>
       </c>
-      <c r="G32" s="74"/>
+      <c r="G32" s="78" t="s">
+        <v>21</v>
+      </c>
       <c r="H32" s="57"/>
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
@@ -2571,7 +2585,7 @@
         <v>92</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="J34" s="20"/>
       <c r="K34" s="32"/>
@@ -2740,6 +2754,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AW2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:Y2"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="N8:O8"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
     <mergeCell ref="N23:O23"/>
     <mergeCell ref="N24:O24"/>
     <mergeCell ref="N25:O25"/>
@@ -2756,22 +2786,6 @@
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N16:O16"/>
     <mergeCell ref="N17:O17"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="AD2:AG2"/>
-    <mergeCell ref="AH2:AW2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:Y2"/>
-    <mergeCell ref="Z2:AC2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="N8:O8"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>